<commit_message>
add mech.dat data to xlsx and sorted. Moved cti files to sub-folder (not used)
</commit_message>
<xml_diff>
--- a/mechfile_comparison.xlsx
+++ b/mechfile_comparison.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,23 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\logan\Desktop\Capstone\Converge\WorkingFiles\CompareContrast_mechfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{103A495C-D8E6-434C-AD85-9C06E3A07689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C53438-1843-4AA8-AA2F-FAE39C48E741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mechfile_comparison" sheetId="1" r:id="rId1"/>
     <sheet name="fromSourcePapers" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">mechfile_comparison!$A$1:$F$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">mechfile_comparison!$A$1:$E$51</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="38">
   <si>
     <t>RXN</t>
   </si>
@@ -98,9 +98,6 @@
     <t>Hong</t>
   </si>
   <si>
-    <t>k ¼ ATn exp(Ea/ RT) in units of [s1 ], [cm3 mol1 s1 ] or [cm6 mol2 s1 ].</t>
-  </si>
-  <si>
     <t>Units are cm3 mol s cal K; k = AT n exp(–Ea /RT)</t>
   </si>
   <si>
@@ -113,13 +110,40 @@
     <t>sandiego</t>
   </si>
   <si>
-    <t>k ¼ BTn exp(Ta/T)</t>
+    <t>O+H2O=OH+OH</t>
+  </si>
+  <si>
+    <t>O2+M=O+O+M</t>
+  </si>
+  <si>
+    <t>OH+M=O+H+M</t>
+  </si>
+  <si>
+    <t>H2O2+O2=HO2+HO2</t>
+  </si>
+  <si>
+    <t>H2O2+H=H2+HO2</t>
+  </si>
+  <si>
+    <t>H2O2+OH=H2O+HO2</t>
+  </si>
+  <si>
+    <t>mech.dat from converge</t>
+  </si>
+  <si>
+    <t>converge mech.dat native file</t>
+  </si>
+  <si>
+    <t>k = ATn exp(Ea/ RT) in units of [s1 ], [cm3 mol1 s1 ] or [cm6 mol2 s1 ].</t>
+  </si>
+  <si>
+    <t>k = BTn exp(Ta/T)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -662,6 +686,54 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>563104</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F35A48B-DB0A-3F88-53E9-CC7E7B5525D5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect b="35330"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9858375" y="2028825"/>
+          <a:ext cx="8087854" cy="1343025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1114,645 +1186,921 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1">
+        <v>6.366E+20</v>
+      </c>
+      <c r="C2">
+        <v>-1.72</v>
+      </c>
+      <c r="D2">
+        <v>524.79999999999995</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2.65E+19</v>
+      </c>
+      <c r="C3">
+        <v>-1.3</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1">
+        <v>5.75E+19</v>
+      </c>
+      <c r="C4">
+        <v>-1.4</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1">
+        <v>5.75E+19</v>
+      </c>
+      <c r="C5">
+        <v>-1.4</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1475000000000</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>104000000000000</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>15286</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1">
+        <v>104000000000000</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>15286</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1">
+        <v>191500000000000</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>16440</v>
+      </c>
+      <c r="E9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1">
+        <v>4.577E+19</v>
+      </c>
+      <c r="C10">
+        <v>-1.4</v>
+      </c>
+      <c r="D10" s="1">
+        <v>104380</v>
+      </c>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+      <c r="K10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1">
+        <v>5.84E+18</v>
+      </c>
+      <c r="C11">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="D11" s="1">
+        <v>104380</v>
+      </c>
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1">
+        <v>4.577E+19</v>
+      </c>
+      <c r="C12">
+        <v>-1.4</v>
+      </c>
+      <c r="D12" s="1">
+        <v>104400</v>
+      </c>
+      <c r="E12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="1">
+        <v>6.0640000000000002E+27</v>
+      </c>
+      <c r="C13">
+        <v>-3.3220000000000001</v>
+      </c>
+      <c r="D13" s="1">
+        <v>120790</v>
+      </c>
+      <c r="E13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="1">
+        <v>6.0599999999999999E+27</v>
+      </c>
+      <c r="C14">
+        <v>-3.31</v>
+      </c>
+      <c r="D14" s="1">
+        <v>120770</v>
+      </c>
+      <c r="E14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1.9120000000000001E+23</v>
+      </c>
+      <c r="C15">
+        <v>-1.83</v>
+      </c>
+      <c r="D15" s="1">
+        <v>118500</v>
+      </c>
+      <c r="E15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1">
+        <v>2.49E+24</v>
+      </c>
+      <c r="C16">
+        <v>-2.2999999999999998</v>
+      </c>
+      <c r="D16" s="1">
+        <v>48749</v>
+      </c>
+      <c r="E16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="1">
+        <v>295100000000000</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1">
+        <v>48430</v>
+      </c>
+      <c r="E17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="1">
+        <v>60250000000000</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1">
+        <v>7950</v>
+      </c>
+      <c r="E18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="1">
+        <v>24100000000000</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>3970</v>
+      </c>
+      <c r="E19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="1">
+        <v>10200000000000</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>3577</v>
+      </c>
+      <c r="E20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="1">
+        <v>10000000000000</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>3585.09</v>
+      </c>
+      <c r="E21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="1">
+        <v>10000000000000</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>3585.09</v>
+      </c>
+      <c r="E22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="1">
+        <v>24100000000000</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0</v>
+      </c>
+      <c r="D23" s="1">
+        <v>3970</v>
+      </c>
+      <c r="E23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="1">
+        <v>9550000</v>
+      </c>
+      <c r="C24">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="1">
-        <v>6.366E+20</v>
-      </c>
-      <c r="D2">
-        <v>-1.72</v>
-      </c>
-      <c r="E2">
-        <v>524.79999999999995</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="D24">
+        <v>3970</v>
+      </c>
+      <c r="E24" t="s">
         <v>6</v>
       </c>
-      <c r="L2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>16</v>
       </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1">
-        <v>2.65E+19</v>
-      </c>
-      <c r="D3">
-        <v>-1.3</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="B25" s="1">
+        <v>843000000000</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>3970</v>
+      </c>
+      <c r="E25" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" s="1">
+        <v>9550000</v>
+      </c>
+      <c r="C26" s="1">
+        <v>2</v>
+      </c>
+      <c r="D26" s="1">
+        <v>3970</v>
+      </c>
+      <c r="E26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="1">
+        <v>4.634E+16</v>
+      </c>
+      <c r="C27" s="1">
+        <v>-0.35</v>
+      </c>
+      <c r="D27" s="1">
+        <v>50670</v>
+      </c>
+      <c r="E27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="1">
+        <v>14340000000000</v>
+      </c>
+      <c r="C28" s="1">
+        <v>-0.35</v>
+      </c>
+      <c r="D28" s="1">
+        <v>37060</v>
+      </c>
+      <c r="E28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1000000000000</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0</v>
+      </c>
+      <c r="E29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="1">
+        <v>580000000000000</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0</v>
+      </c>
+      <c r="D30" s="1">
+        <v>9557</v>
+      </c>
+      <c r="E30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" s="1">
+        <v>2750000</v>
+      </c>
+      <c r="C31">
+        <v>2.09</v>
+      </c>
+      <c r="D31">
+        <v>-1451</v>
+      </c>
+      <c r="E31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="1">
+        <v>16600000000000</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>822.9</v>
+      </c>
+      <c r="E32" t="s">
         <v>19</v>
       </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1">
-        <v>5.75E+19</v>
-      </c>
-      <c r="D4">
-        <v>-1.4</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4" t="s">
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" s="1">
+        <v>16600000000000</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>822.9</v>
+      </c>
+      <c r="E33" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34" s="1">
+        <v>16600000000000</v>
+      </c>
+      <c r="C34" s="1">
+        <v>0</v>
+      </c>
+      <c r="D34" s="1">
+        <v>823</v>
+      </c>
+      <c r="E34" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" s="1">
+        <v>70790000000000</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>295</v>
+      </c>
+      <c r="E35" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" s="1">
+        <v>70790000000000</v>
+      </c>
+      <c r="C36" s="1">
+        <v>0</v>
+      </c>
+      <c r="D36" s="1">
+        <v>295</v>
+      </c>
+      <c r="E36" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37" s="1">
+        <v>20000000000000</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37" t="s">
         <v>19</v>
       </c>
-      <c r="L4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>24</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="1">
-        <v>5.75E+19</v>
-      </c>
-      <c r="D5">
-        <v>-1.4</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5" t="s">
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38" s="1">
+        <v>20000000000000</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38" t="s">
         <v>21</v>
       </c>
-      <c r="L5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>0</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1">
-        <v>104000000000000</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6" s="1">
-        <v>15286</v>
-      </c>
-      <c r="F6" t="s">
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>20</v>
+      </c>
+      <c r="B39" s="1">
+        <v>32500000000000</v>
+      </c>
+      <c r="C39" s="1">
+        <v>0</v>
+      </c>
+      <c r="D39" s="1">
+        <v>0</v>
+      </c>
+      <c r="E39" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>13</v>
+      </c>
+      <c r="B40" s="1">
+        <v>28900000000000</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>-497</v>
+      </c>
+      <c r="E40" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="1">
-        <v>104000000000000</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7" s="1">
-        <v>15286</v>
-      </c>
-      <c r="F7" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41" s="1">
+        <v>7000000000000</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>-1094.6500000000001</v>
+      </c>
+      <c r="E41" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>13</v>
+      </c>
+      <c r="B42" s="1">
+        <v>7000000000000</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>-1094.6500000000001</v>
+      </c>
+      <c r="E42" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>13</v>
+      </c>
+      <c r="B43" s="1">
+        <v>28900000000000</v>
+      </c>
+      <c r="C43" s="1">
+        <v>0</v>
+      </c>
+      <c r="D43" s="1">
+        <v>-497</v>
+      </c>
+      <c r="E43" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" s="1">
+        <v>3818000000000</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>7948</v>
+      </c>
+      <c r="E44" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" s="1">
+        <v>3820000000000</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>7948</v>
+      </c>
+      <c r="E45" t="s">
         <v>17</v>
       </c>
-      <c r="L7" t="s">
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46" s="1">
+        <v>50800</v>
+      </c>
+      <c r="C46">
+        <v>2.67</v>
+      </c>
+      <c r="D46" s="1">
+        <v>6292</v>
+      </c>
+      <c r="E46" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="1">
-        <v>4.577E+19</v>
-      </c>
-      <c r="D8">
-        <v>-1.4</v>
-      </c>
-      <c r="E8" s="1">
-        <v>104380</v>
-      </c>
-      <c r="F8" t="s">
-        <v>6</v>
-      </c>
-      <c r="L8" t="s">
+      <c r="B47" s="1">
+        <v>2970000</v>
+      </c>
+      <c r="C47">
+        <v>2.02</v>
+      </c>
+      <c r="D47" s="1">
+        <v>13400</v>
+      </c>
+      <c r="E47" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="1">
-        <v>5.84E+18</v>
-      </c>
-      <c r="D9">
-        <v>-1.1000000000000001</v>
-      </c>
-      <c r="E9" s="1">
-        <v>104380</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="B48" s="1">
+        <v>4.515E+17</v>
+      </c>
+      <c r="C48" s="1">
+        <v>-0.64</v>
+      </c>
+      <c r="D48" s="1">
+        <v>118900</v>
+      </c>
+      <c r="E48" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>18</v>
+      </c>
+      <c r="B49" s="1">
+        <v>217000000</v>
+      </c>
+      <c r="C49">
+        <v>1.52</v>
+      </c>
+      <c r="D49">
+        <v>3457</v>
+      </c>
+      <c r="E49" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>3</v>
-      </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="1">
-        <v>6.0640000000000002E+27</v>
-      </c>
-      <c r="D10">
-        <v>-3.3220000000000001</v>
-      </c>
-      <c r="E10" s="1">
-        <v>120790</v>
-      </c>
-      <c r="F10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>15</v>
-      </c>
-      <c r="B11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="1">
-        <v>6.0599999999999999E+27</v>
-      </c>
-      <c r="D11">
-        <v>-3.31</v>
-      </c>
-      <c r="E11" s="1">
-        <v>120770</v>
-      </c>
-      <c r="F11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>8</v>
-      </c>
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="1">
-        <v>2.49E+24</v>
-      </c>
-      <c r="D12">
-        <v>-2.2999999999999998</v>
-      </c>
-      <c r="E12" s="1">
-        <v>48749</v>
-      </c>
-      <c r="F12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>9</v>
-      </c>
-      <c r="B13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="1">
-        <v>24100000000000</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>3970</v>
-      </c>
-      <c r="F13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>17</v>
-      </c>
-      <c r="B14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="1">
-        <v>10200000000000</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>3577</v>
-      </c>
-      <c r="F14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>23</v>
-      </c>
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="1">
-        <v>10000000000000</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>3585.09</v>
-      </c>
-      <c r="F15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>28</v>
-      </c>
-      <c r="B16" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="1">
-        <v>10000000000000</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>3585.09</v>
-      </c>
-      <c r="F16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>10</v>
-      </c>
-      <c r="B17" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="1">
-        <v>9550000</v>
-      </c>
-      <c r="D17">
-        <v>2</v>
-      </c>
-      <c r="E17">
-        <v>3970</v>
-      </c>
-      <c r="F17" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>18</v>
       </c>
-      <c r="B18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="1">
-        <v>843000000000</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>3970</v>
-      </c>
-      <c r="F18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>5</v>
-      </c>
-      <c r="B19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="1">
-        <v>2750000</v>
-      </c>
-      <c r="D19">
-        <v>2.09</v>
-      </c>
-      <c r="E19">
-        <v>-1451</v>
-      </c>
-      <c r="F19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>20</v>
-      </c>
-      <c r="B20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="1">
-        <v>16600000000000</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>822.9</v>
-      </c>
-      <c r="F20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>25</v>
-      </c>
-      <c r="B21" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="1">
-        <v>16600000000000</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>822.9</v>
-      </c>
-      <c r="F21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>6</v>
-      </c>
-      <c r="B22" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" s="1">
-        <v>70790000000000</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>295</v>
-      </c>
-      <c r="F22" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="1">
-        <v>20000000000000</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>26</v>
-      </c>
-      <c r="B24" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" s="1">
-        <v>20000000000000</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>7</v>
-      </c>
-      <c r="B25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="1">
-        <v>28900000000000</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <v>-497</v>
-      </c>
-      <c r="F25" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>22</v>
-      </c>
-      <c r="B26" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" s="1">
-        <v>7000000000000</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <v>-1094.6500000000001</v>
-      </c>
-      <c r="F26" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>27</v>
-      </c>
-      <c r="B27" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="1">
-        <v>7000000000000</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>-1094.6500000000001</v>
-      </c>
-      <c r="F27" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>1</v>
-      </c>
-      <c r="B28" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" s="1">
-        <v>3818000000000</v>
-      </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <v>7948</v>
-      </c>
-      <c r="F28" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>12</v>
-      </c>
-      <c r="B29" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" s="1">
-        <v>3820000000000</v>
-      </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>7948</v>
-      </c>
-      <c r="F29" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>13</v>
-      </c>
-      <c r="B30" t="s">
-        <v>18</v>
-      </c>
-      <c r="C30" s="1">
-        <v>217000000</v>
-      </c>
-      <c r="D30">
-        <v>1.52</v>
-      </c>
-      <c r="E30">
-        <v>3457</v>
-      </c>
-      <c r="F30" t="s">
-        <v>17</v>
+      <c r="B50" s="1">
+        <v>216000000</v>
+      </c>
+      <c r="C50">
+        <v>1.51</v>
+      </c>
+      <c r="D50" s="1">
+        <v>3430</v>
+      </c>
+      <c r="E50" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>30</v>
+      </c>
+      <c r="B51" s="1">
+        <v>9.88E+17</v>
+      </c>
+      <c r="C51" s="1">
+        <v>0.74</v>
+      </c>
+      <c r="D51" s="1">
+        <v>102100</v>
+      </c>
+      <c r="E51" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F30">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F30">
-      <sortCondition ref="B1:B30"/>
+  <autoFilter ref="A1:E51" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E51">
+      <sortCondition ref="A1:A51"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB1"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
@@ -1763,7 +2111,7 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1774,7 +2122,7 @@
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="K1" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
@@ -1786,7 +2134,7 @@
       <c r="S1" s="2"/>
       <c r="T1" s="2"/>
       <c r="V1" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>

</xml_diff>